<commit_message>
made an exe file
</commit_message>
<xml_diff>
--- a/Python_Practice/Python_GUI/Py-to-xl/people.xlsx
+++ b/Python_Practice/Python_GUI/Py-to-xl/people.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
@@ -1488,6 +1488,26 @@
         </is>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Rishi</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>20</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Subscribed</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>